<commit_message>
Update Crud & get by email
</commit_message>
<xml_diff>
--- a/System Tasks.xlsx
+++ b/System Tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\DEVOP Soloution\System Hr Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{536DF108-3E73-4C05-841B-C929EC1F97D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C2645CC-CBBF-4919-A1F5-D5D954643EDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{EDAD0D49-344F-45E7-ADA1-6962A3EE362F}"/>
   </bookViews>
@@ -89,9 +89,6 @@
     <t>Implement Service to fetch data from the backend API.</t>
   </si>
   <si>
-    <t>Design UI for displaying employee details (e.g., table with pagination and search filters).</t>
-  </si>
-  <si>
     <t>As a normal employee, I want to view my own details so that I can track my vacation balance and request off days.</t>
   </si>
   <si>
@@ -168,6 +165,9 @@
   </si>
   <si>
     <t>Create Employee List Component to display employee details(Full Name, Role , Vacation Balance)</t>
+  </si>
+  <si>
+    <t>Design UI for displaying employee details.</t>
   </si>
 </sst>
 </file>
@@ -191,7 +191,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -201,6 +201,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -217,7 +223,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -242,6 +248,7 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -578,8 +585,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F75BA76-94A1-4958-82A9-8186A5559AE0}">
   <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -604,10 +611,10 @@
         <v>11</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
@@ -624,7 +631,7 @@
         <v>13</v>
       </c>
       <c r="E2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -640,7 +647,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -651,16 +658,18 @@
         <v>15</v>
       </c>
       <c r="E4" t="s">
-        <v>39</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="F4" s="10"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C5" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>43</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="F5" s="10"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C6" s="3" t="s">
@@ -669,14 +678,16 @@
       <c r="D6" s="8" t="s">
         <v>16</v>
       </c>
+      <c r="F6" s="10"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C7" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>17</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="F7" s="10"/>
     </row>
     <row r="8" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -684,16 +695,16 @@
         <v>1</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>19</v>
-      </c>
       <c r="E9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -701,10 +712,10 @@
         <v>7</v>
       </c>
       <c r="D10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -712,16 +723,18 @@
         <v>8</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>21</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="F11" s="10"/>
     </row>
     <row r="12" spans="1:6" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C12" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>22</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="F12" s="10"/>
     </row>
     <row r="13" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="14" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -729,16 +742,16 @@
         <v>2</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -746,10 +759,10 @@
         <v>7</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -757,7 +770,7 @@
         <v>8</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
@@ -766,16 +779,16 @@
         <v>3</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
@@ -783,10 +796,10 @@
         <v>7</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E19" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
@@ -794,10 +807,10 @@
         <v>7</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
@@ -806,24 +819,24 @@
         <v>4</v>
       </c>
       <c r="B22" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C22" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="E22" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C23" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="24" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
@@ -832,16 +845,16 @@
         <v>5</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
@@ -849,10 +862,10 @@
         <v>7</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E26" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
@@ -860,7 +873,7 @@
         <v>8</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>